<commit_message>
Group Vertical account calculation and total
</commit_message>
<xml_diff>
--- a/src/Tests/pickles/change_worksheet_output.xlsx
+++ b/src/Tests/pickles/change_worksheet_output.xlsx
@@ -492,6 +492,25 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
@@ -1207,6 +1226,25 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1"/>
@@ -3376,6 +3414,25 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1"/>

</xml_diff>